<commit_message>
figures with black fonts
</commit_message>
<xml_diff>
--- a/2019_neurips_vigil/results/Results paper VIGIL_v16.xlsx
+++ b/2019_neurips_vigil/results/Results paper VIGIL_v16.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentalbouy/Desktop/COG_publications/2019_neurips_vigil/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszkornuta/Documents/GitHub/COG_publications/2019_neurips_vigil/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C8BB185-4C75-344D-BB2A-3BA2BE454F4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB28BD16-E29A-0D4C-9BC1-C36FEEEF11C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{3D9B9DCB-639E-0F40-9945-E2955BC58740}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{3D9B9DCB-639E-0F40-9945-E2955BC58740}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="66">
   <si>
     <t xml:space="preserve">Trained on </t>
   </si>
@@ -208,22 +211,28 @@
     <t>COG (Paper)</t>
   </si>
   <si>
-    <t>Canonical</t>
-  </si>
-  <si>
-    <t>Hard</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Training</t>
   </si>
   <si>
     <t>Finetuning</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Canonical-Canonical</t>
+  </si>
+  <si>
+    <t>Canonical-Hard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Hard-Hard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>(Fine-tuning)</t>
   </si>
 </sst>
 </file>
@@ -766,7 +775,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1344,7 +1353,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1650,17 +1659,7 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.4678653997296064E-2"/>
-          <c:y val="1.0738349879469701E-2"/>
-          <c:w val="0.93589276801780696"/>
-          <c:h val="0.86638001304519774"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1668,6 +1667,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>SAMNet</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1695,10 +1697,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="bg1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1737,76 +1736,177 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet1!$P$41:$R$43</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="3"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Canonical</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Canonical</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Canonical</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Hard</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Canonical</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Hard</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Hard</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>Sheet1!$A$15:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>AndCompareColor</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AndCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AndSimpleCompareColor</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AndSimpleCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CompareColor</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CompareShape</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Exist</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ExistColor</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>ExistColorOf</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>ExistColorSpace</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>ExistLastColorSameShape</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ExistLastObjectSameObject</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>ExistLastShapeSameColor</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ExistShape</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>ExistShapeOf</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ExistShapeSpace</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>ExistSpace</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>GetColor</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>GetColorSpace</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>GetShape</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>GetShapeSpace</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>SimpleCompareShape</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>SimpleCompareColor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$41:$S$43</c:f>
+              <c:f>Sheet1!$D$15:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>0.97991424800000004</c:v>
+                  <c:v>0.93489399939999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91630190609999995</c:v>
+                  <c:v>0.93200639259999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.96685707570000001</c:v>
+                  <c:v>0.99196963739999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99248780709999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98118233160000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9804640107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99971400919999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99975800770000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99945901449999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94067396640000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9945441746</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97268610249999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98160858849999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99402324819999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.93500411809999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.95311949240000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99988277219999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.97992283869999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99990595540000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.97484548670000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99938934170000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99981246629999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-156F-0047-AFEE-0F86259CAF4E}"/>
+              <c16:uniqueId val="{00000000-E14F-2442-9D7D-975FE97B6C6B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>COG</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1831,10 +1931,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1872,68 +1969,87 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet1!$P$41:$R$43</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="3"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Canonical</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Canonical</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Canonical</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>N/A</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Hard</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Canonical</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Hard</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Hard</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$41:$T$43</c:f>
+              <c:f>Sheet1!$T$15:$T$37</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>0.96699999999999997</c:v>
+                  <c:v>0.81871342659000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65900000000000003</c:v>
+                  <c:v>0.79989439249000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78100000000000003</c:v>
+                  <c:v>0.99659228324899995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99206250906000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99404764175399996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98958331346499995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99691176414500005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98882681131399996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98016309738200003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98378378152799995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98863637447399999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98170733451799996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98113209009199998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-156F-0047-AFEE-0F86259CAF4E}"/>
+              <c16:uniqueId val="{00000001-E14F-2442-9D7D-975FE97B6C6B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1945,8 +2061,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="20"/>
         <c:axId val="1113063551"/>
         <c:axId val="1238457167"/>
       </c:barChart>
@@ -1955,45 +2070,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1238457167"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
@@ -2006,7 +2088,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.4"/>
+          <c:min val="0.70000000000000007"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2083,12 +2165,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2204,163 +2281,65 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$15:$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>AndCompareColor</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>AndCompareShape</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>AndSimpleCompareColor</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>AndSimpleCompareShape</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>CompareColor</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CompareShape</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Exist</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ExistColor</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>ExistColorOf</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>ExistColorSpace</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>ExistLastColorSameShape</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>ExistLastObjectSameObject</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>ExistLastShapeSameColor</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>ExistShape</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>ExistShapeOf</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>ExistShapeSpace</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>ExistSpace</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>GetColor</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>GetColorSpace</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>GetShape</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>GetShapeSpace</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>SimpleCompareShape</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>SimpleCompareColor</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$Q$41:$R$44</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Canonical-Canonical</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Canonical-Hard</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Canonical-Hard</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Hard-Hard</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v> </c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v> </c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>(Fine-tuning)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>   </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$15:$D$37</c:f>
+              <c:f>[1]Sheet1!$S$41:$S$44</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.93489399939999995</c:v>
+                  <c:v>0.97991424800000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93200639259999996</c:v>
+                  <c:v>0.91630190609999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99196963739999999</c:v>
+                  <c:v>0.96685707570000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99248780709999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.98118233160000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.9804640107</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.99971400919999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.99975800770000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.99945901449999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.94067396640000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9945441746</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.97268610249999998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.98160858849999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.99402324819999999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.93500411809999995</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.95311949240000005</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.99988277219999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.97992283869999997</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.99990595540000005</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.97484548670000004</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.99938934170000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.99981246629999998</c:v>
+                  <c:v>0.96124106649999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E14F-2442-9D7D-975FE97B6C6B}"/>
+              <c16:uniqueId val="{00000000-359E-2E47-AB49-16A29988B0C8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2368,12 +2347,12 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>COG</c:v>
+            <c:v>COG (Ours)</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="bg1">
-                <a:lumMod val="75000"/>
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -2437,87 +2416,193 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$Q$41:$R$44</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Canonical-Canonical</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Canonical-Hard</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Canonical-Hard</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Hard-Hard</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v> </c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v> </c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>(Fine-tuning)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>   </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$15:$T$37</c:f>
+              <c:f>[1]Sheet1!$T$41:$T$44</c:f>
               <c:numCache>
-                <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.81871342659000002</c:v>
+                  <c:v>0.96699999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.79989439249000005</c:v>
+                  <c:v>0.65900000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99659228324899995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.99206250906000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.99404764175399996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.98958331346499995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.99691176414500005</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.98882681131399996</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.98016309738200003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.98378378152799995</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.98863637447399999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.98170733451799996</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.98113209009199998</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>0.78100000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E14F-2442-9D7D-975FE97B6C6B}"/>
+              <c16:uniqueId val="{00000001-359E-2E47-AB49-16A29988B0C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>COG (Paper)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$Q$41:$R$44</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Canonical-Canonical</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Canonical-Hard</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Canonical-Hard</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Hard-Hard</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v> </c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v> </c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>(Fine-tuning)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>   </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Sheet1!$U$41:$U$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.0%">
+                  <c:v>0.97599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00%">
+                  <c:v>0.80100000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-359E-2E47-AB49-16A29988B0C8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2538,12 +2623,45 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="1238457167"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
@@ -2556,7 +2674,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.70000000000000007"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4906,44 +5024,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>327215</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>99358</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F4725A-29E7-9B44-B2B7-6B1AE174AFA5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>103911</xdr:colOff>
       <xdr:row>60</xdr:row>
@@ -4974,6 +5054,44 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF1C0037-8F5E-F94C-9550-D6B62292A70E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
@@ -4981,6 +5099,93 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="41">
+          <cell r="P41" t="str">
+            <v>Canonical</v>
+          </cell>
+          <cell r="Q41" t="str">
+            <v>N/A</v>
+          </cell>
+          <cell r="R41" t="str">
+            <v>Canonical</v>
+          </cell>
+          <cell r="S41">
+            <v>0.97991424800000004</v>
+          </cell>
+          <cell r="T41">
+            <v>0.96699999999999997</v>
+          </cell>
+          <cell r="U41">
+            <v>0.97599999999999998</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="P42" t="str">
+            <v>Hard</v>
+          </cell>
+          <cell r="Q42" t="str">
+            <v>N/A</v>
+          </cell>
+          <cell r="R42" t="str">
+            <v>Canonical</v>
+          </cell>
+          <cell r="S42">
+            <v>0.91630190609999995</v>
+          </cell>
+          <cell r="T42">
+            <v>0.65900000000000003</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="P43" t="str">
+            <v>Hard</v>
+          </cell>
+          <cell r="Q43" t="str">
+            <v>Hard</v>
+          </cell>
+          <cell r="R43" t="str">
+            <v>Canonical</v>
+          </cell>
+          <cell r="S43">
+            <v>0.96685707570000001</v>
+          </cell>
+          <cell r="T43">
+            <v>0.78100000000000003</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="P44" t="str">
+            <v>Hard</v>
+          </cell>
+          <cell r="Q44" t="str">
+            <v>N/A</v>
+          </cell>
+          <cell r="R44" t="str">
+            <v>Hard</v>
+          </cell>
+          <cell r="S44">
+            <v>0.96124106649999996</v>
+          </cell>
+          <cell r="U44">
+            <v>0.80100000000000005</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7639,13 +7844,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="N8:Q8"/>
     <mergeCell ref="K4:L4"/>
@@ -7655,6 +7853,13 @@
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7664,8 +7869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F950B3BD-F67F-7347-9596-8AB8CAAAC726}">
   <dimension ref="A1:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M33" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="U44" sqref="U44"/>
+    <sheetView tabSelected="1" topLeftCell="N36" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9995,14 +10200,11 @@
       <c r="J40" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="P40" t="s">
-        <v>63</v>
-      </c>
       <c r="Q40" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="R40" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="S40" t="s">
         <v>55</v>
@@ -10016,14 +10218,11 @@
     </row>
     <row r="41" spans="1:30">
       <c r="A41" s="1"/>
-      <c r="P41" t="s">
-        <v>58</v>
-      </c>
       <c r="Q41" t="s">
+        <v>64</v>
+      </c>
+      <c r="R41" t="s">
         <v>60</v>
-      </c>
-      <c r="R41" t="s">
-        <v>58</v>
       </c>
       <c r="S41" s="37">
         <f>D13</f>
@@ -10040,14 +10239,11 @@
     </row>
     <row r="42" spans="1:30">
       <c r="A42" s="1"/>
-      <c r="P42" t="s">
-        <v>59</v>
-      </c>
       <c r="Q42" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="R42" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="S42" s="37">
         <f>G13</f>
@@ -10060,14 +10256,11 @@
     </row>
     <row r="43" spans="1:30">
       <c r="A43" s="1"/>
-      <c r="P43" t="s">
-        <v>59</v>
-      </c>
       <c r="Q43" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="R43" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="S43" s="37">
         <f>J13</f>
@@ -10080,8 +10273,20 @@
     </row>
     <row r="44" spans="1:30">
       <c r="A44" s="1"/>
-      <c r="S44" s="37"/>
-      <c r="U44" s="40"/>
+      <c r="Q44" t="s">
+        <v>62</v>
+      </c>
+      <c r="R44" t="s">
+        <v>63</v>
+      </c>
+      <c r="S44" s="37">
+        <f>P13</f>
+        <v>0.96124106649999996</v>
+      </c>
+      <c r="U44" s="40">
+        <f>W13</f>
+        <v>0.80100000000000005</v>
+      </c>
     </row>
     <row r="45" spans="1:30">
       <c r="A45" s="1"/>

</xml_diff>